<commit_message>
Vari update (maggiori dettagli in descrizione)
- Inserito scenario alternativo per connessione a database
- Aggiornate tabelle di tracciamento e dei requisiti
- Aggiornato foglio di calcolo contenente i riferimenti
- Inserito attore Rocket.Chat su casi d'uso di interazione grafica
- Aggiornati i diagrammi dei casi d'uso per il punto sopra
- Aggiornato diario delle modifiche
</commit_message>
<xml_diff>
--- a/LaTex/documenti/AnalisiDeiRequisiti/label_requisiti-uc.xlsx
+++ b/LaTex/documenti/AnalisiDeiRequisiti/label_requisiti-uc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Riferimenti per Req" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="406">
   <si>
     <t>impostazioni</t>
   </si>
@@ -1229,6 +1229,15 @@
   </si>
   <si>
     <t>L109</t>
+  </si>
+  <si>
+    <t>UC1.00.2</t>
+  </si>
+  <si>
+    <t>2,1,1</t>
+  </si>
+  <si>
+    <t>2,1,2</t>
   </si>
 </sst>
 </file>
@@ -2083,8 +2092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L153"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2287,7 +2296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2298,7 +2307,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2309,7 +2318,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2320,7 +2329,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2331,7 +2340,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2342,7 +2351,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2353,7 +2362,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2364,7 +2373,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2375,7 +2384,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2386,7 +2395,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2397,7 +2406,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2408,7 +2417,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2419,7 +2428,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2430,7 +2439,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2438,28 +2447,31 @@
         <v>387</v>
       </c>
       <c r="C30" t="s">
+        <v>403</v>
+      </c>
+      <c r="D30" t="s">
         <v>170</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>171</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>174</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>175</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>176</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>177</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2470,7 +2482,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3727,10 +3739,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N159"/>
+  <dimension ref="A1:N160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3787,8 +3799,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>2.1</v>
+      <c r="A6" s="1" t="s">
+        <v>404</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -3806,28 +3818,25 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>294</v>
+        <v>405</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>403</v>
       </c>
       <c r="C7">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B7)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" t="s">
-        <v>88</v>
+        <v>387</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B8)</f>
@@ -3837,672 +3846,685 @@
         <v>86</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>378</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B9)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>379</v>
+        <v>86</v>
+      </c>
+      <c r="E9" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>222</v>
+        <v>378</v>
       </c>
       <c r="C10">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B10)</f>
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>238</v>
+        <v>297</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>222</v>
       </c>
       <c r="C11">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B11)</f>
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C12">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B12)</f>
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B13)</f>
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B14)</f>
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B15)</f>
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B16)</f>
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B17)</f>
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B18)</f>
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C19">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B19)</f>
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>298</v>
+        <v>246</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B20)</f>
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>247</v>
+        <v>298</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C21">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B21)</f>
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>170</v>
+        <v>14</v>
       </c>
       <c r="C22">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B22)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>381</v>
-      </c>
-      <c r="E22" t="s">
-        <v>387</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="C23">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B23)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>381</v>
+      </c>
+      <c r="E23" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="C24">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B24)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>382</v>
-      </c>
-      <c r="E24" t="s">
-        <v>387</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>19</v>
+        <v>171</v>
       </c>
       <c r="C25">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B25)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>100</v>
+        <v>382</v>
+      </c>
+      <c r="E25" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C26">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B26)</f>
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C27">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B27)</f>
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B28)</f>
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>172</v>
+        <v>17</v>
       </c>
       <c r="C29">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B29)</f>
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C30">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B30)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" t="s">
-        <v>383</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C31">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B31)</f>
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>387</v>
+        <v>82</v>
       </c>
       <c r="E31" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>174</v>
       </c>
       <c r="C32">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B32)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>114</v>
+        <v>387</v>
+      </c>
+      <c r="E32" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>175</v>
+        <v>34</v>
       </c>
       <c r="C33">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B33)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>387</v>
-      </c>
-      <c r="E33" t="s">
-        <v>385</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="C34">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B34)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>103</v>
+        <v>387</v>
+      </c>
+      <c r="E34" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C35">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B35)</f>
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>386</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="C36">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B36)</f>
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>118</v>
+        <v>386</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B37)</f>
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C38">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B38)</f>
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C39">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B39)</f>
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C40">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B40)</f>
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C41">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B41)</f>
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C42">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B42)</f>
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C43">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B43)</f>
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>176</v>
+        <v>25</v>
       </c>
       <c r="C44">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B44)</f>
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>387</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>28</v>
+        <v>176</v>
       </c>
       <c r="C45">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B45)</f>
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>108</v>
+        <v>387</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
       <c r="C46">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B46)</f>
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>387</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="C47">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B47)</f>
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>107</v>
+        <v>387</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>178</v>
+        <v>27</v>
       </c>
       <c r="C48">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B48)</f>
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>387</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="C49">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B49)</f>
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>106</v>
+        <v>387</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C50">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B50)</f>
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C51">
         <f>COUNTIF('Riferimenti per Req'!C:Z,B51)</f>
         <v>1</v>
       </c>
       <c r="D51" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52">
+        <f>COUNTIF('Riferimenti per Req'!C:Z,B52)</f>
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -4510,14 +4532,7 @@
         <v>278</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C54">
-        <f>COUNTIF('Riferimenti per Req'!C:K,B54)</f>
-        <v>1</v>
-      </c>
-      <c r="D54" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -4525,14 +4540,14 @@
         <v>279</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C55">
         <f>COUNTIF('Riferimenti per Req'!C:K,B55)</f>
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -4540,14 +4555,14 @@
         <v>280</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>179</v>
+        <v>43</v>
       </c>
       <c r="C56">
         <f>COUNTIF('Riferimenti per Req'!C:K,B56)</f>
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>388</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -4555,14 +4570,14 @@
         <v>281</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>44</v>
+        <v>179</v>
       </c>
       <c r="C57">
         <f>COUNTIF('Riferimenti per Req'!C:K,B57)</f>
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>131</v>
+        <v>388</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -4570,14 +4585,14 @@
         <v>282</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C58">
         <f>COUNTIF('Riferimenti per Req'!C:K,B58)</f>
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -4585,17 +4600,14 @@
         <v>283</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="C59">
         <f>COUNTIF('Riferimenti per Req'!C:K,B59)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>133</v>
-      </c>
-      <c r="E59" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -4603,14 +4615,17 @@
         <v>284</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>181</v>
+        <v>45</v>
       </c>
       <c r="C60">
         <f>COUNTIF('Riferimenti per Req'!C:K,B60)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D60" t="s">
         <v>133</v>
+      </c>
+      <c r="E60" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -4618,14 +4633,14 @@
         <v>285</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C61">
         <f>COUNTIF('Riferimenti per Req'!C:K,B61)</f>
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>388</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -4633,14 +4648,14 @@
         <v>286</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C62">
         <f>COUNTIF('Riferimenti per Req'!C:K,B62)</f>
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>131</v>
+        <v>388</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -4648,14 +4663,14 @@
         <v>287</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C63">
         <f>COUNTIF('Riferimenti per Req'!C:K,B63)</f>
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -4663,17 +4678,14 @@
         <v>288</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>46</v>
+        <v>184</v>
       </c>
       <c r="C64">
         <f>COUNTIF('Riferimenti per Req'!C:K,B64)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>135</v>
-      </c>
-      <c r="E64" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -4681,17 +4693,17 @@
         <v>289</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C65">
         <f>COUNTIF('Riferimenti per Req'!C:K,B65)</f>
         <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E65" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -4699,14 +4711,17 @@
         <v>290</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>185</v>
+        <v>47</v>
       </c>
       <c r="C66">
         <f>COUNTIF('Riferimenti per Req'!C:K,B66)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D66" t="s">
         <v>137</v>
+      </c>
+      <c r="E66" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -4714,14 +4729,14 @@
         <v>291</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C67">
         <f>COUNTIF('Riferimenti per Req'!C:K,B67)</f>
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>388</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -4729,14 +4744,14 @@
         <v>292</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C68">
         <f>COUNTIF('Riferimenti per Req'!C:K,B68)</f>
         <v>1</v>
       </c>
       <c r="D68" t="s">
-        <v>131</v>
+        <v>388</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -4744,19 +4759,26 @@
         <v>293</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C69">
         <f>COUNTIF('Riferimenti per Req'!C:K,B69)</f>
         <v>1</v>
       </c>
       <c r="D69" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C70">
+        <f>COUNTIF('Riferimenti per Req'!C:K,B70)</f>
+        <v>1</v>
+      </c>
+      <c r="D70" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -4764,14 +4786,7 @@
         <v>299</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C72">
-        <f>COUNTIF('Riferimenti per Req'!C:K,B72)</f>
-        <v>1</v>
-      </c>
-      <c r="D72" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -4779,14 +4794,14 @@
         <v>300</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>197</v>
+        <v>51</v>
       </c>
       <c r="C73">
         <f>COUNTIF('Riferimenti per Req'!C:K,B73)</f>
         <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>389</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -4794,14 +4809,14 @@
         <v>301</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C74">
         <f>COUNTIF('Riferimenti per Req'!C:K,B74)</f>
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -4809,14 +4824,14 @@
         <v>302</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C75">
         <f>COUNTIF('Riferimenti per Req'!C:K,B75)</f>
         <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -4824,17 +4839,14 @@
         <v>304</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="C76">
         <f>COUNTIF('Riferimenti per Req'!C:K,B76)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D76" t="s">
-        <v>143</v>
-      </c>
-      <c r="E76" t="s">
-        <v>144</v>
+        <v>391</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -4842,14 +4854,17 @@
         <v>310</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C77">
         <f>COUNTIF('Riferimenti per Req'!C:K,B77)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D77" t="s">
-        <v>140</v>
+        <v>143</v>
+      </c>
+      <c r="E77" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -4857,17 +4872,14 @@
         <v>303</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>189</v>
+        <v>56</v>
       </c>
       <c r="C78">
         <f>COUNTIF('Riferimenti per Req'!C:K,B78)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>143</v>
-      </c>
-      <c r="E78" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -4875,23 +4887,17 @@
         <v>311</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>53</v>
+        <v>189</v>
       </c>
       <c r="C79">
         <f>COUNTIF('Riferimenti per Req'!C:K,B79)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E79" t="s">
-        <v>146</v>
-      </c>
-      <c r="F79" t="s">
-        <v>147</v>
-      </c>
-      <c r="G79" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -4899,14 +4905,23 @@
         <v>312</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>190</v>
+        <v>53</v>
       </c>
       <c r="C80">
         <f>COUNTIF('Riferimenti per Req'!C:K,B80)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D80" t="s">
         <v>145</v>
+      </c>
+      <c r="E80" t="s">
+        <v>146</v>
+      </c>
+      <c r="F80" t="s">
+        <v>147</v>
+      </c>
+      <c r="G80" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -4914,7 +4929,7 @@
         <v>305</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C81">
         <f>COUNTIF('Riferimenti per Req'!C:K,B81)</f>
@@ -4929,14 +4944,14 @@
         <v>313</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C82">
         <f>COUNTIF('Riferimenti per Req'!C:K,B82)</f>
         <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>392</v>
+        <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -4944,14 +4959,14 @@
         <v>314</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>223</v>
+        <v>192</v>
       </c>
       <c r="C83">
         <f>COUNTIF('Riferimenti per Req'!C:K,B83)</f>
         <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -4959,14 +4974,14 @@
         <v>315</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C84">
         <f>COUNTIF('Riferimenti per Req'!C:K,B84)</f>
         <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -4974,14 +4989,14 @@
         <v>316</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="C85">
         <f>COUNTIF('Riferimenti per Req'!C:K,B85)</f>
         <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>139</v>
+        <v>391</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -4989,14 +5004,14 @@
         <v>317</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C86">
         <f>COUNTIF('Riferimenti per Req'!C:K,B86)</f>
         <v>1</v>
       </c>
       <c r="D86" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -5004,7 +5019,7 @@
         <v>318</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C87">
         <f>COUNTIF('Riferimenti per Req'!C:K,B87)</f>
@@ -5019,19 +5034,26 @@
         <v>319</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>48</v>
+        <v>202</v>
       </c>
       <c r="C88">
         <f>COUNTIF('Riferimenti per Req'!C:K,B88)</f>
         <v>1</v>
       </c>
       <c r="D88" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C89">
+        <f>COUNTIF('Riferimenti per Req'!C:K,B89)</f>
+        <v>1</v>
+      </c>
+      <c r="D89" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -5039,14 +5061,7 @@
         <v>320</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C91">
-        <f>COUNTIF('Riferimenti per Req'!C:K,B91)</f>
-        <v>1</v>
-      </c>
-      <c r="D91" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -5054,14 +5069,14 @@
         <v>321</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C92">
         <f>COUNTIF('Riferimenti per Req'!C:K,B92)</f>
         <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -5069,14 +5084,14 @@
         <v>322</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>203</v>
+        <v>57</v>
       </c>
       <c r="C93">
         <f>COUNTIF('Riferimenti per Req'!C:K,B93)</f>
         <v>1</v>
       </c>
       <c r="D93" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -5084,17 +5099,14 @@
         <v>323</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>55</v>
+        <v>203</v>
       </c>
       <c r="C94">
         <f>COUNTIF('Riferimenti per Req'!C:K,B94)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D94" t="s">
-        <v>150</v>
-      </c>
-      <c r="E94" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -5102,14 +5114,17 @@
         <v>324</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>204</v>
+        <v>55</v>
       </c>
       <c r="C95">
         <f>COUNTIF('Riferimenti per Req'!C:K,B95)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D95" t="s">
         <v>150</v>
+      </c>
+      <c r="E95" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -5117,19 +5132,26 @@
         <v>325</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>62</v>
+        <v>204</v>
       </c>
       <c r="C96">
         <f>COUNTIF('Riferimenti per Req'!C:K,B96)</f>
         <v>1</v>
       </c>
       <c r="D96" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C97">
+        <f>COUNTIF('Riferimenti per Req'!C:K,B97)</f>
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -5137,14 +5159,7 @@
         <v>326</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C99">
-        <f>COUNTIF('Riferimenti per Req'!C:K,B99)</f>
-        <v>1</v>
-      </c>
-      <c r="D99" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -5152,14 +5167,14 @@
         <v>327</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C100">
         <f>COUNTIF('Riferimenti per Req'!C:K,B100)</f>
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -5167,14 +5182,14 @@
         <v>328</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>205</v>
+        <v>59</v>
       </c>
       <c r="C101">
         <f>COUNTIF('Riferimenti per Req'!C:K,B101)</f>
         <v>1</v>
       </c>
       <c r="D101" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -5182,14 +5197,14 @@
         <v>329</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>80</v>
+        <v>205</v>
       </c>
       <c r="C102">
         <f>COUNTIF('Riferimenti per Req'!C:K,B102)</f>
         <v>1</v>
       </c>
       <c r="D102" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -5197,7 +5212,7 @@
         <v>330</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>206</v>
+        <v>80</v>
       </c>
       <c r="C103">
         <f>COUNTIF('Riferimenti per Req'!C:K,B103)</f>
@@ -5212,14 +5227,14 @@
         <v>331</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>64</v>
+        <v>206</v>
       </c>
       <c r="C104">
         <f>COUNTIF('Riferimenti per Req'!C:K,B104)</f>
         <v>1</v>
       </c>
       <c r="D104" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -5227,14 +5242,14 @@
         <v>332</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C105">
         <f>COUNTIF('Riferimenti per Req'!C:K,B105)</f>
         <v>1</v>
       </c>
       <c r="D105" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -5242,7 +5257,7 @@
         <v>333</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>207</v>
+        <v>81</v>
       </c>
       <c r="C106">
         <f>COUNTIF('Riferimenti per Req'!C:K,B106)</f>
@@ -5257,19 +5272,26 @@
         <v>334</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>65</v>
+        <v>207</v>
       </c>
       <c r="C107">
         <f>COUNTIF('Riferimenti per Req'!C:K,B107)</f>
         <v>1</v>
       </c>
       <c r="D107" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C108">
+        <f>COUNTIF('Riferimenti per Req'!C:K,B108)</f>
+        <v>1</v>
+      </c>
+      <c r="D108" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -5277,14 +5299,7 @@
         <v>335</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C110">
-        <f>COUNTIF('Riferimenti per Req'!C:K,B110)</f>
-        <v>1</v>
-      </c>
-      <c r="D110" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -5292,14 +5307,14 @@
         <v>336</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C111">
         <f>COUNTIF('Riferimenti per Req'!C:K,B111)</f>
         <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -5307,14 +5322,14 @@
         <v>337</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>208</v>
+        <v>58</v>
       </c>
       <c r="C112">
         <f>COUNTIF('Riferimenti per Req'!C:K,B112)</f>
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -5322,14 +5337,14 @@
         <v>338</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>71</v>
+        <v>208</v>
       </c>
       <c r="C113">
         <f>COUNTIF('Riferimenti per Req'!C:K,B113)</f>
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -5337,7 +5352,7 @@
         <v>339</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>209</v>
+        <v>71</v>
       </c>
       <c r="C114">
         <f>COUNTIF('Riferimenti per Req'!C:K,B114)</f>
@@ -5352,19 +5367,26 @@
         <v>340</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>63</v>
+        <v>209</v>
       </c>
       <c r="C115">
         <f>COUNTIF('Riferimenti per Req'!C:K,B115)</f>
         <v>1</v>
       </c>
       <c r="D115" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C116">
+        <f>COUNTIF('Riferimenti per Req'!C:K,B116)</f>
+        <v>1</v>
+      </c>
+      <c r="D116" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -5372,14 +5394,7 @@
         <v>341</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C118">
-        <f>COUNTIF('Riferimenti per Req'!C:K,B118)</f>
-        <v>1</v>
-      </c>
-      <c r="D118" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -5387,14 +5402,14 @@
         <v>342</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>210</v>
+        <v>76</v>
       </c>
       <c r="C119">
-        <f>COUNTIF('Riferimenti per Req'!C:L,B119)</f>
+        <f>COUNTIF('Riferimenti per Req'!C:K,B119)</f>
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -5402,14 +5417,14 @@
         <v>343</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C120">
         <f>COUNTIF('Riferimenti per Req'!C:L,B120)</f>
         <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -5417,14 +5432,14 @@
         <v>306</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>74</v>
+        <v>211</v>
       </c>
       <c r="C121">
         <f>COUNTIF('Riferimenti per Req'!C:L,B121)</f>
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>394</v>
+        <v>157</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -5432,14 +5447,14 @@
         <v>344</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>212</v>
+        <v>74</v>
       </c>
       <c r="C122">
         <f>COUNTIF('Riferimenti per Req'!C:L,B122)</f>
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -5447,14 +5462,14 @@
         <v>345</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C123">
         <f>COUNTIF('Riferimenti per Req'!C:L,B123)</f>
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -5462,14 +5477,14 @@
         <v>346</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C124">
         <f>COUNTIF('Riferimenti per Req'!C:L,B124)</f>
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>139</v>
+        <v>396</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -5477,14 +5492,14 @@
         <v>349</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C125">
         <f>COUNTIF('Riferimenti per Req'!C:L,B125)</f>
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>398</v>
+        <v>139</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -5492,14 +5507,14 @@
         <v>347</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C126">
         <f>COUNTIF('Riferimenti per Req'!C:L,B126)</f>
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -5507,14 +5522,14 @@
         <v>350</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>60</v>
+        <v>225</v>
       </c>
       <c r="C127">
         <f>COUNTIF('Riferimenti per Req'!C:L,B127)</f>
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>140</v>
+        <v>397</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -5522,14 +5537,14 @@
         <v>351</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>226</v>
+        <v>60</v>
       </c>
       <c r="C128">
         <f>COUNTIF('Riferimenti per Req'!C:L,B128)</f>
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>397</v>
+        <v>140</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -5537,17 +5552,14 @@
         <v>352</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C129">
         <f>COUNTIF('Riferimenti per Req'!C:L,B129)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>398</v>
-      </c>
-      <c r="E129" t="s">
-        <v>156</v>
+        <v>397</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -5555,14 +5567,17 @@
         <v>353</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C130">
         <f>COUNTIF('Riferimenti per Req'!C:L,B130)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D130" t="s">
-        <v>399</v>
+        <v>398</v>
+      </c>
+      <c r="E130" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -5570,14 +5585,14 @@
         <v>354</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C131">
         <f>COUNTIF('Riferimenti per Req'!C:L,B131)</f>
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -5585,14 +5600,14 @@
         <v>355</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>66</v>
+        <v>228</v>
       </c>
       <c r="C132">
         <f>COUNTIF('Riferimenti per Req'!C:L,B132)</f>
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>141</v>
+        <v>395</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -5600,17 +5615,14 @@
         <v>307</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C133">
         <f>COUNTIF('Riferimenti per Req'!C:L,B133)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>398</v>
-      </c>
-      <c r="E133" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -5618,14 +5630,17 @@
         <v>356</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>230</v>
+        <v>72</v>
       </c>
       <c r="C134">
         <f>COUNTIF('Riferimenti per Req'!C:L,B134)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D134" t="s">
-        <v>399</v>
+        <v>398</v>
+      </c>
+      <c r="E134" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -5633,14 +5648,14 @@
         <v>357</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C135">
         <f>COUNTIF('Riferimenti per Req'!C:L,B135)</f>
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -5648,14 +5663,14 @@
         <v>358</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C136">
         <f>COUNTIF('Riferimenti per Req'!C:L,B136)</f>
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>139</v>
+        <v>400</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -5663,14 +5678,14 @@
         <v>359</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>193</v>
+        <v>232</v>
       </c>
       <c r="C137">
         <f>COUNTIF('Riferimenti per Req'!C:L,B137)</f>
         <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>396</v>
+        <v>139</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -5678,14 +5693,14 @@
         <v>360</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>67</v>
+        <v>193</v>
       </c>
       <c r="C138">
         <f>COUNTIF('Riferimenti per Req'!C:L,B138)</f>
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>141</v>
+        <v>396</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -5693,17 +5708,14 @@
         <v>361</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C139">
         <f>COUNTIF('Riferimenti per Req'!C:L,B139)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>398</v>
-      </c>
-      <c r="E139" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -5711,14 +5723,17 @@
         <v>362</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>194</v>
+        <v>73</v>
       </c>
       <c r="C140">
         <f>COUNTIF('Riferimenti per Req'!C:L,B140)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D140" t="s">
-        <v>401</v>
+        <v>398</v>
+      </c>
+      <c r="E140" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -5726,14 +5741,14 @@
         <v>363</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C141">
         <f>COUNTIF('Riferimenti per Req'!C:L,B141)</f>
         <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>390</v>
+        <v>401</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -5741,14 +5756,14 @@
         <v>364</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C142">
         <f>COUNTIF('Riferimenti per Req'!C:L,B142)</f>
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -5756,14 +5771,14 @@
         <v>365</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>68</v>
+        <v>196</v>
       </c>
       <c r="C143">
         <f>COUNTIF('Riferimenti per Req'!C:L,B143)</f>
         <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>141</v>
+        <v>391</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -5771,14 +5786,14 @@
         <v>366</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C144">
         <f>COUNTIF('Riferimenti per Req'!C:L,B144)</f>
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.25">
@@ -5786,14 +5801,14 @@
         <v>348</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="C145">
         <f>COUNTIF('Riferimenti per Req'!C:L,B145)</f>
         <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
@@ -5801,14 +5816,14 @@
         <v>367</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>216</v>
+        <v>61</v>
       </c>
       <c r="C146">
         <f>COUNTIF('Riferimenti per Req'!C:L,B146)</f>
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.25">
@@ -5816,14 +5831,14 @@
         <v>308</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C147">
         <f>COUNTIF('Riferimenti per Req'!C:L,B147)</f>
         <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>401</v>
+        <v>158</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.25">
@@ -5831,14 +5846,14 @@
         <v>368</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C148">
         <f>COUNTIF('Riferimenti per Req'!C:L,B148)</f>
         <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>390</v>
+        <v>401</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.25">
@@ -5846,14 +5861,14 @@
         <v>369</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C149">
         <f>COUNTIF('Riferimenti per Req'!C:L,B149)</f>
         <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.25">
@@ -5861,14 +5876,14 @@
         <v>370</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>69</v>
+        <v>219</v>
       </c>
       <c r="C150">
         <f>COUNTIF('Riferimenti per Req'!C:L,B150)</f>
         <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>141</v>
+        <v>391</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
@@ -5876,14 +5891,14 @@
         <v>371</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C151">
         <f>COUNTIF('Riferimenti per Req'!C:L,B151)</f>
         <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.25">
@@ -5891,14 +5906,14 @@
         <v>372</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C152">
         <f>COUNTIF('Riferimenti per Req'!C:L,B152)</f>
         <v>1</v>
       </c>
       <c r="D152" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.25">
@@ -5906,14 +5921,14 @@
         <v>373</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="C153">
         <f>COUNTIF('Riferimenti per Req'!C:L,B153)</f>
         <v>1</v>
       </c>
       <c r="D153" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.25">
@@ -5921,17 +5936,14 @@
         <v>309</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>220</v>
+        <v>75</v>
       </c>
       <c r="C154">
         <f>COUNTIF('Riferimenti per Req'!C:L,B154)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D154" t="s">
-        <v>399</v>
-      </c>
-      <c r="E154" t="s">
-        <v>402</v>
+        <v>158</v>
       </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.25">
@@ -5939,14 +5951,17 @@
         <v>374</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C155">
         <f>COUNTIF('Riferimenti per Req'!C:L,B155)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D155" t="s">
-        <v>395</v>
+        <v>399</v>
+      </c>
+      <c r="E155" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.25">
@@ -5954,67 +5969,79 @@
         <v>375</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>50</v>
+        <v>221</v>
       </c>
       <c r="C156">
         <f>COUNTIF('Riferimenti per Req'!C:L,B156)</f>
         <v>1</v>
       </c>
       <c r="D156" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B157" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C157">
+        <f>COUNTIF('Riferimenti per Req'!C:L,B157)</f>
+        <v>1</v>
+      </c>
+      <c r="D157" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B158" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D158" t="s">
-        <v>1</v>
-      </c>
-      <c r="E158" t="s">
-        <v>4</v>
-      </c>
-      <c r="F158" t="s">
-        <v>83</v>
-      </c>
-      <c r="G158" t="s">
-        <v>121</v>
-      </c>
-      <c r="H158" t="s">
-        <v>122</v>
-      </c>
-      <c r="I158" t="s">
-        <v>123</v>
-      </c>
-      <c r="J158" t="s">
-        <v>124</v>
-      </c>
-      <c r="K158" t="s">
-        <v>125</v>
-      </c>
-      <c r="L158" t="s">
-        <v>126</v>
-      </c>
-      <c r="M158" t="s">
-        <v>127</v>
-      </c>
-      <c r="N158" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B159" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D159" t="s">
+        <v>1</v>
+      </c>
+      <c r="E159" t="s">
+        <v>4</v>
+      </c>
+      <c r="F159" t="s">
+        <v>83</v>
+      </c>
+      <c r="G159" t="s">
+        <v>121</v>
+      </c>
+      <c r="H159" t="s">
+        <v>122</v>
+      </c>
+      <c r="I159" t="s">
+        <v>123</v>
+      </c>
+      <c r="J159" t="s">
+        <v>124</v>
+      </c>
+      <c r="K159" t="s">
+        <v>125</v>
+      </c>
+      <c r="L159" t="s">
+        <v>126</v>
+      </c>
+      <c r="M159" t="s">
+        <v>127</v>
+      </c>
+      <c r="N159" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B160" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D160" t="s">
         <v>82</v>
       </c>
-      <c r="E159" t="s">
+      <c r="E160" t="s">
         <v>86</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C54:C69 C72:C88 C91:C96 C99:C107 C110:C115 C118:C1048576 C4:C51">
+  <conditionalFormatting sqref="C55:C70 C73:C89 C92:C97 C100:C108 C111:C116 C119:C1048576 C4:C52">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>